<commit_message>
adding patterns to the map
</commit_message>
<xml_diff>
--- a/Plot Work/1917 Victory Map/Victory Map of 1917 State Types.xlsx
+++ b/Plot Work/1917 Victory Map/Victory Map of 1917 State Types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RBY11\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5781B0-6891-4526-AA12-959C0F051ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0298525-4197-4F41-BF02-226C100B1A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10455" yWindow="825" windowWidth="21600" windowHeight="11835" xr2:uid="{DA0E77D7-1B92-4340-9A8D-E4AF89B9DC01}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="110">
   <si>
     <t>State</t>
   </si>
@@ -353,6 +353,18 @@
   </si>
   <si>
     <t>Connecticut</t>
+  </si>
+  <si>
+    <t>circle</t>
+  </si>
+  <si>
+    <t>stripe</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -704,15 +716,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC3D07F-35FF-460F-9A33-7A00C188A41D}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -722,8 +734,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -733,8 +748,11 @@
       <c r="C2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -744,8 +762,11 @@
       <c r="C3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -755,8 +776,11 @@
       <c r="C4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -766,8 +790,11 @@
       <c r="C5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -777,8 +804,11 @@
       <c r="C6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -788,8 +818,11 @@
       <c r="C7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -799,8 +832,11 @@
       <c r="C8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -810,8 +846,11 @@
       <c r="C9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -821,8 +860,11 @@
       <c r="C10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -832,8 +874,11 @@
       <c r="C11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -843,8 +888,11 @@
       <c r="C12" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -854,8 +902,11 @@
       <c r="C13" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -865,8 +916,11 @@
       <c r="C14" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -876,8 +930,11 @@
       <c r="C15" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -887,8 +944,11 @@
       <c r="C16" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -898,8 +958,11 @@
       <c r="C17" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -909,8 +972,11 @@
       <c r="C18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -920,8 +986,11 @@
       <c r="C19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -931,8 +1000,11 @@
       <c r="C20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -942,8 +1014,11 @@
       <c r="C21" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -953,8 +1028,11 @@
       <c r="C22" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -964,8 +1042,11 @@
       <c r="C23" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -975,8 +1056,11 @@
       <c r="C24" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -986,8 +1070,11 @@
       <c r="C25" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -997,8 +1084,11 @@
       <c r="C26" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1008,8 +1098,11 @@
       <c r="C27" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1019,8 +1112,11 @@
       <c r="C28" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1030,8 +1126,11 @@
       <c r="C29" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1041,8 +1140,11 @@
       <c r="C30" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1052,8 +1154,11 @@
       <c r="C31" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1063,8 +1168,11 @@
       <c r="C32" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1074,8 +1182,11 @@
       <c r="C33" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1085,8 +1196,11 @@
       <c r="C34" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1096,8 +1210,11 @@
       <c r="C35" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1107,8 +1224,11 @@
       <c r="C36" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1118,8 +1238,11 @@
       <c r="C37" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -1129,8 +1252,11 @@
       <c r="C38" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1140,8 +1266,11 @@
       <c r="C39" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1151,8 +1280,11 @@
       <c r="C40" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1162,8 +1294,11 @@
       <c r="C41" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1173,8 +1308,11 @@
       <c r="C42" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -1184,8 +1322,11 @@
       <c r="C43" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1195,8 +1336,11 @@
       <c r="C44" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1206,8 +1350,11 @@
       <c r="C45" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -1217,8 +1364,11 @@
       <c r="C46" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1228,8 +1378,11 @@
       <c r="C47" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1239,8 +1392,11 @@
       <c r="C48" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1249,6 +1405,9 @@
       </c>
       <c r="C49" t="s">
         <v>103</v>
+      </c>
+      <c r="D49" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>